<commit_message>
EMEAA REGION EXCEL UPDATES
</commit_message>
<xml_diff>
--- a/emeaa-v1.xlsx
+++ b/emeaa-v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\backupRoy\Documents\26470\excel-reader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0A3C01-EA5C-41A0-8049-A53070EC7391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A8CCF4-562E-4C2A-92B5-5EC9808CF0B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="602" firstSheet="4" activeTab="5" xr2:uid="{A20E3CA5-7A46-443B-849E-145CA743A390}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="602" firstSheet="5" activeTab="10" xr2:uid="{A20E3CA5-7A46-443B-849E-145CA743A390}"/>
   </bookViews>
   <sheets>
     <sheet name="Colour Guide" sheetId="14" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4747" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4744" uniqueCount="194">
   <si>
     <t>Brand</t>
   </si>
@@ -1017,7 +1017,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1311,6 +1311,9 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1840,8 +1843,8 @@
   </sheetPr>
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3896,6 +3899,7 @@
     <hyperlink ref="B35" r:id="rId34" xr:uid="{DA9CEDF8-AA3D-411A-A548-91BDB20FA6DC}"/>
     <hyperlink ref="B36" r:id="rId35" xr:uid="{AC13D020-8D35-42BB-A150-1FD0C9C5AB1D}"/>
     <hyperlink ref="B4" r:id="rId36" xr:uid="{4341C55E-EDDB-488B-BCD7-C93900687E97}"/>
+    <hyperlink ref="B37" r:id="rId37" xr:uid="{AC89402D-F696-4CA5-970A-861D8DC51978}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3906,10 +3910,10 @@
   <sheetPr>
     <tabColor rgb="FF404040"/>
   </sheetPr>
-  <dimension ref="A1:R41"/>
+  <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4012,240 +4016,238 @@
       <c r="R2" s="2"/>
     </row>
     <row r="3" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>68</v>
+      <c r="A3" s="48" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" s="49" t="s">
+        <v>178</v>
       </c>
       <c r="C3" s="15"/>
-      <c r="D3" s="16" t="s">
-        <v>64</v>
-      </c>
+      <c r="D3" s="16"/>
       <c r="E3" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J3" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K3" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L3" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M3" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N3" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O3" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P3" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q3" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R3" s="2"/>
     </row>
     <row r="4" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="48" t="s">
-        <v>176</v>
-      </c>
-      <c r="B4" s="49" t="s">
-        <v>178</v>
-      </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="16"/>
+      <c r="A4" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="28"/>
+      <c r="D4" s="16" t="s">
+        <v>73</v>
+      </c>
       <c r="E4" s="12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F4" s="12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G4" s="12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H4" s="12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I4" s="12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J4" s="12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K4" s="12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L4" s="12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M4" s="12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N4" s="12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="O4" s="12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P4" s="12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Q4" s="12">
-        <v>1</v>
-      </c>
-      <c r="R4" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="R4" s="3"/>
     </row>
     <row r="5" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
         <v>71</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C5" s="28"/>
       <c r="D5" s="16" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E5" s="12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F5" s="12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G5" s="12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H5" s="12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I5" s="12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J5" s="12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K5" s="12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L5" s="12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M5" s="12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N5" s="12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O5" s="12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P5" s="12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q5" s="12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R5" s="3"/>
     </row>
     <row r="6" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C6" s="28"/>
-      <c r="D6" s="16" t="s">
-        <v>75</v>
-      </c>
+      <c r="D6" s="16"/>
       <c r="E6" s="12">
-        <v>5</v>
-      </c>
-      <c r="F6" s="12">
-        <v>5</v>
-      </c>
-      <c r="G6" s="12">
-        <v>5</v>
-      </c>
-      <c r="H6" s="12">
-        <v>5</v>
-      </c>
-      <c r="I6" s="12">
-        <v>5</v>
-      </c>
-      <c r="J6" s="12">
-        <v>5</v>
-      </c>
-      <c r="K6" s="12">
-        <v>5</v>
-      </c>
-      <c r="L6" s="12">
-        <v>5</v>
-      </c>
-      <c r="M6" s="12">
-        <v>5</v>
-      </c>
-      <c r="N6" s="12">
-        <v>5</v>
-      </c>
-      <c r="O6" s="12">
-        <v>5</v>
-      </c>
-      <c r="P6" s="12">
-        <v>5</v>
-      </c>
-      <c r="Q6" s="12">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="O6" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="P6" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q6" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="R6" s="3"/>
     </row>
     <row r="7" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="C7" s="28"/>
+        <v>79</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="15"/>
       <c r="D7" s="16"/>
       <c r="E7" s="12">
+        <v>7</v>
+      </c>
+      <c r="F7" s="12">
         <v>6</v>
       </c>
-      <c r="F7" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="K7" s="12" t="s">
-        <v>78</v>
+      <c r="G7" s="12">
+        <v>6</v>
+      </c>
+      <c r="H7" s="12">
+        <v>6</v>
+      </c>
+      <c r="I7" s="12">
+        <v>6</v>
+      </c>
+      <c r="J7" s="12">
+        <v>6</v>
+      </c>
+      <c r="K7" s="12">
+        <v>6</v>
       </c>
       <c r="L7" s="12" t="s">
         <v>78</v>
@@ -4259,43 +4261,43 @@
       <c r="O7" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="P7" s="12" t="s">
-        <v>78</v>
+      <c r="P7" s="12">
+        <v>6</v>
       </c>
       <c r="Q7" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="R7" s="3"/>
+      <c r="R7" s="2"/>
     </row>
     <row r="8" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" s="15"/>
+        <v>81</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="16"/>
       <c r="D8" s="16"/>
       <c r="E8" s="12">
+        <v>8</v>
+      </c>
+      <c r="F8" s="12">
         <v>7</v>
       </c>
-      <c r="F8" s="12">
-        <v>6</v>
-      </c>
       <c r="G8" s="12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H8" s="12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I8" s="12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J8" s="12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K8" s="12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L8" s="12" t="s">
         <v>78</v>
@@ -4310,7 +4312,7 @@
         <v>78</v>
       </c>
       <c r="P8" s="12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q8" s="12" t="s">
         <v>78</v>
@@ -4319,444 +4321,446 @@
     </row>
     <row r="9" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
+        <v>83</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="16" t="s">
+        <v>64</v>
+      </c>
       <c r="E9" s="12">
+        <v>9</v>
+      </c>
+      <c r="F9" s="12">
         <v>8</v>
       </c>
-      <c r="F9" s="12">
+      <c r="G9" s="12">
+        <v>8</v>
+      </c>
+      <c r="H9" s="12">
+        <v>8</v>
+      </c>
+      <c r="I9" s="12">
+        <v>8</v>
+      </c>
+      <c r="J9" s="12">
+        <v>8</v>
+      </c>
+      <c r="K9" s="12">
+        <v>8</v>
+      </c>
+      <c r="L9" s="12">
+        <v>6</v>
+      </c>
+      <c r="M9" s="12">
+        <v>6</v>
+      </c>
+      <c r="N9" s="12">
+        <v>6</v>
+      </c>
+      <c r="O9" s="12">
+        <v>6</v>
+      </c>
+      <c r="P9" s="12">
+        <v>8</v>
+      </c>
+      <c r="Q9" s="12">
+        <v>6</v>
+      </c>
+      <c r="R9" s="2"/>
+    </row>
+    <row r="10" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="26"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="12">
+        <v>10</v>
+      </c>
+      <c r="F10" s="12">
+        <v>9</v>
+      </c>
+      <c r="G10" s="12">
+        <v>9</v>
+      </c>
+      <c r="H10" s="12">
+        <v>9</v>
+      </c>
+      <c r="I10" s="12">
+        <v>9</v>
+      </c>
+      <c r="J10" s="12">
+        <v>9</v>
+      </c>
+      <c r="K10" s="12">
+        <v>9</v>
+      </c>
+      <c r="L10" s="12">
         <v>7</v>
       </c>
-      <c r="G9" s="12">
+      <c r="M10" s="12">
         <v>7</v>
       </c>
-      <c r="H9" s="12">
+      <c r="N10" s="12">
         <v>7</v>
       </c>
-      <c r="I9" s="12">
+      <c r="O10" s="12">
         <v>7</v>
       </c>
-      <c r="J9" s="12">
+      <c r="P10" s="12">
+        <v>9</v>
+      </c>
+      <c r="Q10" s="12">
         <v>7</v>
-      </c>
-      <c r="K9" s="12">
-        <v>7</v>
-      </c>
-      <c r="L9" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="M9" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="N9" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="O9" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="P9" s="12">
-        <v>7</v>
-      </c>
-      <c r="Q9" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="R9" s="2"/>
-    </row>
-    <row r="10" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="12">
-        <v>9</v>
-      </c>
-      <c r="F10" s="12">
-        <v>8</v>
-      </c>
-      <c r="G10" s="12">
-        <v>8</v>
-      </c>
-      <c r="H10" s="12">
-        <v>8</v>
-      </c>
-      <c r="I10" s="12">
-        <v>8</v>
-      </c>
-      <c r="J10" s="12">
-        <v>8</v>
-      </c>
-      <c r="K10" s="12">
-        <v>8</v>
-      </c>
-      <c r="L10" s="12">
-        <v>6</v>
-      </c>
-      <c r="M10" s="12">
-        <v>6</v>
-      </c>
-      <c r="N10" s="12">
-        <v>6</v>
-      </c>
-      <c r="O10" s="12">
-        <v>6</v>
-      </c>
-      <c r="P10" s="12">
-        <v>8</v>
-      </c>
-      <c r="Q10" s="12">
-        <v>6</v>
       </c>
       <c r="R10" s="2"/>
     </row>
     <row r="11" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C11" s="26"/>
       <c r="D11" s="16"/>
       <c r="E11" s="12">
+        <v>11</v>
+      </c>
+      <c r="F11" s="12">
         <v>10</v>
       </c>
-      <c r="F11" s="12">
-        <v>9</v>
-      </c>
       <c r="G11" s="12">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H11" s="12">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I11" s="12">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J11" s="12">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K11" s="12">
-        <v>9</v>
-      </c>
-      <c r="L11" s="12">
-        <v>7</v>
-      </c>
-      <c r="M11" s="12">
-        <v>7</v>
-      </c>
-      <c r="N11" s="12">
-        <v>7</v>
-      </c>
-      <c r="O11" s="12">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="M11" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="N11" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="O11" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="P11" s="12">
-        <v>9</v>
-      </c>
-      <c r="Q11" s="12">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="Q11" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="R11" s="2"/>
     </row>
     <row r="12" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C12" s="26"/>
       <c r="D12" s="16"/>
       <c r="E12" s="12">
+        <v>12</v>
+      </c>
+      <c r="F12" s="12">
         <v>11</v>
       </c>
-      <c r="F12" s="12">
-        <v>10</v>
-      </c>
       <c r="G12" s="12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H12" s="12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I12" s="12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J12" s="12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K12" s="12">
-        <v>10</v>
-      </c>
-      <c r="L12" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="M12" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="N12" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="O12" s="12" t="s">
-        <v>78</v>
+        <v>11</v>
+      </c>
+      <c r="L12" s="12">
+        <v>8</v>
+      </c>
+      <c r="M12" s="12">
+        <v>8</v>
+      </c>
+      <c r="N12" s="12">
+        <v>8</v>
+      </c>
+      <c r="O12" s="12">
+        <v>8</v>
       </c>
       <c r="P12" s="12">
-        <v>10</v>
-      </c>
-      <c r="Q12" s="12" t="s">
-        <v>78</v>
+        <v>11</v>
+      </c>
+      <c r="Q12" s="12">
+        <v>8</v>
       </c>
       <c r="R12" s="2"/>
     </row>
     <row r="13" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C13" s="26"/>
       <c r="D13" s="16"/>
       <c r="E13" s="12">
+        <v>13</v>
+      </c>
+      <c r="F13" s="12">
         <v>12</v>
       </c>
-      <c r="F13" s="12">
-        <v>11</v>
-      </c>
       <c r="G13" s="12">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H13" s="12">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I13" s="12">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J13" s="12">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K13" s="12">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L13" s="12">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M13" s="12">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N13" s="12">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O13" s="12">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="P13" s="12">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q13" s="12">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R13" s="2"/>
     </row>
     <row r="14" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C14" s="26"/>
       <c r="D14" s="16"/>
       <c r="E14" s="12">
+        <v>15</v>
+      </c>
+      <c r="F14" s="12">
+        <v>14</v>
+      </c>
+      <c r="G14" s="12">
         <v>13</v>
       </c>
-      <c r="F14" s="12">
-        <v>12</v>
-      </c>
-      <c r="G14" s="12">
-        <v>12</v>
-      </c>
       <c r="H14" s="12">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I14" s="12">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J14" s="12">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K14" s="12">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="L14" s="12">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M14" s="12">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N14" s="12">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O14" s="12">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="P14" s="12">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="Q14" s="12">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R14" s="2"/>
     </row>
     <row r="15" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C15" s="26"/>
       <c r="D15" s="16"/>
       <c r="E15" s="12">
+        <v>16</v>
+      </c>
+      <c r="F15" s="12">
         <v>15</v>
       </c>
-      <c r="F15" s="12">
+      <c r="G15" s="12">
         <v>14</v>
       </c>
-      <c r="G15" s="12">
-        <v>13</v>
-      </c>
       <c r="H15" s="12">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I15" s="12">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J15" s="12">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K15" s="12">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L15" s="12">
-        <v>10</v>
-      </c>
-      <c r="M15" s="12">
-        <v>10</v>
-      </c>
-      <c r="N15" s="12">
-        <v>10</v>
-      </c>
-      <c r="O15" s="12">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="M15" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="N15" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="O15" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="P15" s="12">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="Q15" s="12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R15" s="2"/>
     </row>
     <row r="16" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C16" s="26"/>
       <c r="D16" s="16"/>
       <c r="E16" s="12">
-        <v>16</v>
-      </c>
-      <c r="F16" s="12">
+        <v>17</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="H16" s="12">
         <v>15</v>
       </c>
-      <c r="G16" s="12">
-        <v>14</v>
-      </c>
-      <c r="H16" s="12">
-        <v>14</v>
-      </c>
-      <c r="I16" s="12">
-        <v>14</v>
-      </c>
-      <c r="J16" s="12">
-        <v>14</v>
-      </c>
-      <c r="K16" s="12">
-        <v>14</v>
+      <c r="I16" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="L16" s="12">
+        <v>12</v>
+      </c>
+      <c r="M16" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="N16" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="O16" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="P16" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q16" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="R16" s="2"/>
+    </row>
+    <row r="17" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="28"/>
+      <c r="D17" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="I17" s="12">
+        <v>15</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="L17" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="M17" s="12">
         <v>11</v>
       </c>
-      <c r="M16" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="N16" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="O16" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="P16" s="12">
-        <v>14</v>
-      </c>
-      <c r="Q16" s="12">
+      <c r="N17" s="12">
         <v>11</v>
-      </c>
-      <c r="R16" s="2"/>
-    </row>
-    <row r="17" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="B17" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="12">
-        <v>17</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="H17" s="12">
-        <v>15</v>
-      </c>
-      <c r="I17" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="J17" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="K17" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="L17" s="12">
-        <v>12</v>
-      </c>
-      <c r="M17" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="N17" s="12" t="s">
-        <v>78</v>
       </c>
       <c r="O17" s="12" t="s">
         <v>78</v>
@@ -4771,90 +4775,88 @@
     </row>
     <row r="18" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C18" s="28"/>
       <c r="D18" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="H18" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="I18" s="12">
+      <c r="E18" s="12">
+        <v>18</v>
+      </c>
+      <c r="F18" s="12">
+        <v>16</v>
+      </c>
+      <c r="G18" s="12">
         <v>15</v>
       </c>
-      <c r="J18" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="K18" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="L18" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="M18" s="12">
+      <c r="H18" s="12">
+        <v>16</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="J18" s="12">
+        <v>15</v>
+      </c>
+      <c r="K18" s="12">
+        <v>15</v>
+      </c>
+      <c r="L18" s="12">
+        <v>13</v>
+      </c>
+      <c r="M18" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="N18" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="O18" s="12">
         <v>11</v>
       </c>
-      <c r="N18" s="12">
-        <v>11</v>
-      </c>
-      <c r="O18" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="P18" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q18" s="12" t="s">
-        <v>78</v>
+      <c r="P18" s="12">
+        <v>15</v>
+      </c>
+      <c r="Q18" s="12">
+        <v>12</v>
       </c>
       <c r="R18" s="2"/>
     </row>
     <row r="19" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C19" s="28"/>
-      <c r="D19" s="16" t="s">
-        <v>64</v>
-      </c>
+      <c r="D19" s="16"/>
       <c r="E19" s="12">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F19" s="12">
+        <v>17</v>
+      </c>
+      <c r="G19" s="12">
         <v>16</v>
       </c>
-      <c r="G19" s="12">
-        <v>15</v>
-      </c>
       <c r="H19" s="12">
+        <v>17</v>
+      </c>
+      <c r="I19" s="12">
         <v>16</v>
       </c>
-      <c r="I19" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="J19" s="12">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K19" s="12">
-        <v>15</v>
-      </c>
-      <c r="L19" s="12">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="L19" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="M19" s="12" t="s">
         <v>78</v>
@@ -4862,46 +4864,46 @@
       <c r="N19" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="O19" s="12">
-        <v>11</v>
+      <c r="O19" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="P19" s="12">
-        <v>15</v>
-      </c>
-      <c r="Q19" s="12">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="Q19" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="R19" s="2"/>
     </row>
     <row r="20" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="B20" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="C20" s="28"/>
+      <c r="A20" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="C20" s="26"/>
       <c r="D20" s="16"/>
       <c r="E20" s="12">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F20" s="12">
+        <v>18</v>
+      </c>
+      <c r="G20" s="12">
         <v>17</v>
       </c>
-      <c r="G20" s="12">
-        <v>16</v>
-      </c>
       <c r="H20" s="12">
-        <v>17</v>
-      </c>
-      <c r="I20" s="12">
-        <v>16</v>
-      </c>
-      <c r="J20" s="12">
-        <v>16</v>
-      </c>
-      <c r="K20" s="12">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="K20" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="L20" s="12" t="s">
         <v>78</v>
@@ -4915,8 +4917,8 @@
       <c r="O20" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="P20" s="12">
-        <v>16</v>
+      <c r="P20" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="Q20" s="12" t="s">
         <v>78</v>
@@ -4925,24 +4927,24 @@
     </row>
     <row r="21" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C21" s="26"/>
       <c r="D21" s="16"/>
       <c r="E21" s="12">
-        <v>20</v>
-      </c>
-      <c r="F21" s="12">
-        <v>18</v>
-      </c>
-      <c r="G21" s="12">
-        <v>17</v>
-      </c>
-      <c r="H21" s="12">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="I21" s="12" t="s">
         <v>78</v>
@@ -4975,15 +4977,15 @@
     </row>
     <row r="22" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C22" s="26"/>
       <c r="D22" s="16"/>
       <c r="E22" s="12">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F22" s="12" t="s">
         <v>78</v>
@@ -5025,15 +5027,15 @@
     </row>
     <row r="23" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C23" s="26"/>
       <c r="D23" s="16"/>
       <c r="E23" s="12">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>78</v>
@@ -5075,15 +5077,15 @@
     </row>
     <row r="24" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C24" s="26"/>
       <c r="D24" s="16"/>
       <c r="E24" s="12">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F24" s="12" t="s">
         <v>78</v>
@@ -5125,24 +5127,24 @@
     </row>
     <row r="25" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C25" s="26"/>
       <c r="D25" s="16"/>
       <c r="E25" s="12">
-        <v>24</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="H25" s="12" t="s">
-        <v>78</v>
+        <v>25</v>
+      </c>
+      <c r="F25" s="12">
+        <v>19</v>
+      </c>
+      <c r="G25" s="12">
+        <v>18</v>
+      </c>
+      <c r="H25" s="12">
+        <v>19</v>
       </c>
       <c r="I25" s="12" t="s">
         <v>78</v>
@@ -5175,24 +5177,24 @@
     </row>
     <row r="26" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C26" s="26"/>
       <c r="D26" s="16"/>
       <c r="E26" s="12">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F26" s="12">
+        <v>20</v>
+      </c>
+      <c r="G26" s="12">
         <v>19</v>
       </c>
-      <c r="G26" s="12">
-        <v>18</v>
-      </c>
       <c r="H26" s="12">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I26" s="12" t="s">
         <v>78</v>
@@ -5225,24 +5227,24 @@
     </row>
     <row r="27" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C27" s="26"/>
-      <c r="D27" s="16"/>
+      <c r="D27" s="60"/>
       <c r="E27" s="12">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F27" s="12">
-        <v>20</v>
-      </c>
-      <c r="G27" s="12">
-        <v>19</v>
-      </c>
-      <c r="H27" s="12">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="I27" s="12" t="s">
         <v>78</v>
@@ -5275,18 +5277,18 @@
     </row>
     <row r="28" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C28" s="26"/>
-      <c r="D28" s="60"/>
+      <c r="D28" s="16"/>
       <c r="E28" s="12">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F28" s="12">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>78</v>
@@ -5325,18 +5327,18 @@
     </row>
     <row r="29" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C29" s="26"/>
-      <c r="D29" s="16"/>
+      <c r="D29" s="60"/>
       <c r="E29" s="12">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F29" s="12">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G29" s="12" t="s">
         <v>78</v>
@@ -5375,18 +5377,18 @@
     </row>
     <row r="30" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="B30" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="C30" s="26"/>
+        <v>125</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="C30" s="15"/>
       <c r="D30" s="60"/>
       <c r="E30" s="12">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F30" s="12">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G30" s="12" t="s">
         <v>78</v>
@@ -5425,21 +5427,21 @@
     </row>
     <row r="31" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="C31" s="15"/>
+        <v>127</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="C31" s="26"/>
       <c r="D31" s="60"/>
       <c r="E31" s="12">
-        <v>30</v>
-      </c>
-      <c r="F31" s="12">
-        <v>24</v>
-      </c>
-      <c r="G31" s="12" t="s">
-        <v>78</v>
+        <v>31</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="G31" s="12">
+        <v>20</v>
       </c>
       <c r="H31" s="12" t="s">
         <v>78</v>
@@ -5475,21 +5477,21 @@
     </row>
     <row r="32" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C32" s="26"/>
       <c r="D32" s="60"/>
       <c r="E32" s="12">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F32" s="12" t="s">
         <v>78</v>
       </c>
       <c r="G32" s="12">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H32" s="12" t="s">
         <v>78</v>
@@ -5525,21 +5527,21 @@
     </row>
     <row r="33" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C33" s="26"/>
-      <c r="D33" s="60"/>
+      <c r="D33" s="16"/>
       <c r="E33" s="12">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>78</v>
       </c>
       <c r="G33" s="12">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H33" s="12" t="s">
         <v>78</v>
@@ -5575,21 +5577,21 @@
     </row>
     <row r="34" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C34" s="26"/>
       <c r="D34" s="16"/>
       <c r="E34" s="12">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F34" s="12" t="s">
         <v>78</v>
       </c>
       <c r="G34" s="12">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H34" s="12" t="s">
         <v>78</v>
@@ -5625,21 +5627,21 @@
     </row>
     <row r="35" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C35" s="26"/>
-      <c r="D35" s="16"/>
+      <c r="D35" s="60"/>
       <c r="E35" s="12">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F35" s="12" t="s">
         <v>78</v>
       </c>
       <c r="G35" s="12">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H35" s="12" t="s">
         <v>78</v>
@@ -5675,21 +5677,21 @@
     </row>
     <row r="36" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C36" s="26"/>
       <c r="D36" s="60"/>
       <c r="E36" s="12">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F36" s="12" t="s">
         <v>78</v>
       </c>
       <c r="G36" s="12">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H36" s="12" t="s">
         <v>78</v>
@@ -5723,23 +5725,23 @@
       </c>
       <c r="R36" s="2"/>
     </row>
-    <row r="37" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C37" s="26"/>
       <c r="D37" s="60"/>
-      <c r="E37" s="12">
-        <v>36</v>
+      <c r="E37" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="F37" s="12" t="s">
         <v>78</v>
       </c>
       <c r="G37" s="12">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H37" s="12" t="s">
         <v>78</v>
@@ -5771,25 +5773,26 @@
       <c r="Q37" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="R37" s="2"/>
-    </row>
-    <row r="38" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="B38" s="26" t="s">
-        <v>140</v>
-      </c>
-      <c r="C38" s="26"/>
-      <c r="D38" s="60"/>
-      <c r="E38" s="12" t="s">
-        <v>78</v>
+    </row>
+    <row r="38" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="E38" s="12">
+        <v>37</v>
       </c>
       <c r="F38" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="G38" s="12">
-        <v>26</v>
+      <c r="G38" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="H38" s="12" t="s">
         <v>78</v>
@@ -5821,20 +5824,21 @@
       <c r="Q38" s="12" t="s">
         <v>78</v>
       </c>
+      <c r="R38" s="2"/>
     </row>
     <row r="39" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="25" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C39" s="17"/>
       <c r="D39" s="17" t="s">
         <v>143</v>
       </c>
       <c r="E39" s="12">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F39" s="12" t="s">
         <v>78</v>
@@ -5874,144 +5878,92 @@
       </c>
       <c r="R39" s="2"/>
     </row>
-    <row r="40" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="B40" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="C40" s="17"/>
-      <c r="D40" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="E40" s="12">
-        <v>38</v>
-      </c>
-      <c r="F40" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="G40" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="H40" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="I40" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="J40" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="K40" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="L40" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="M40" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="N40" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="O40" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="P40" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q40" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="R40" s="2"/>
-    </row>
-    <row r="41" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="50" t="s">
+    <row r="40" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="50" t="s">
         <v>183</v>
       </c>
-      <c r="B41" s="51" t="s">
+      <c r="B40" s="51" t="s">
         <v>184</v>
       </c>
-      <c r="E41" s="92">
+      <c r="E40" s="92">
         <v>14</v>
       </c>
-      <c r="F41" s="92">
+      <c r="F40" s="92">
         <v>13</v>
       </c>
-      <c r="G41" s="92">
+      <c r="G40" s="92">
         <v>13</v>
       </c>
-      <c r="H41" s="92">
+      <c r="H40" s="92">
         <v>13</v>
       </c>
-      <c r="I41" s="92">
+      <c r="I40" s="92">
         <v>13</v>
       </c>
-      <c r="J41" s="92">
+      <c r="J40" s="92">
         <v>13</v>
       </c>
-      <c r="K41" s="92">
+      <c r="K40" s="92">
         <v>13</v>
       </c>
-      <c r="L41" s="92">
+      <c r="L40" s="92">
         <v>10</v>
       </c>
-      <c r="M41" s="92">
+      <c r="M40" s="92">
         <v>10</v>
       </c>
-      <c r="N41" s="92">
+      <c r="N40" s="92">
         <v>10</v>
       </c>
-      <c r="O41" s="92">
+      <c r="O40" s="92">
         <v>10</v>
       </c>
-      <c r="P41" s="92">
+      <c r="P40" s="92">
         <v>13</v>
       </c>
-      <c r="Q41" s="92">
+      <c r="Q40" s="92">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="https://mylearning.sumtotal.host/rcore/c/pillarRedirect?isDeepLink=1&amp;relyingParty=LM&amp;url=https%3A%2F%2Fmylearning.sumtotal.host%2Flearning%2Fcore%2Factivitydetails%2FViewActivityDetails%3FUserMode%3D0%26ActivityId%3D10770%26ClassUnderStruct%3DFalse%26CallerUrl%3D%2Flearning%2Flearner%2FHome%2FGoToPortal%3Fkey%3D0%26SearchCallerURL%3Dhttps%253A%252F%252Fmylearning.sumtotal.host%252Fcore%252FsearchRedirect%253FViewType%253DList%2526SearchText%253Dwelcome%25252520to%25252520ihg%2526startRow%253D0%26SearchCallerID%3D2" xr:uid="{45743D37-33AE-4A36-A4A3-4C2B7B95EAEC}"/>
-    <hyperlink ref="B18" r:id="rId2" xr:uid="{6307E43C-9BC0-489B-9BB5-E5C2004BE1F8}"/>
-    <hyperlink ref="B10" r:id="rId3" display="https://mylearning.sumtotal.host/rcore/c/pillarRedirect?isDeepLink=1&amp;relyingParty=LM&amp;url=https%3A%2F%2Fmylearning.sumtotal.host%2Flearning%2Fcore%2Factivitydetails%2FViewActivityDetails%3FUserMode%3D0%26ActivityId%3D21837%26ClassUnderStruct%3DFalse%26CallerUrl%3D%2Flearning%2Flearner%2FHome%2FGoToPortal%3Fkey%3D0%26SearchCallerURL%3Dhttps%253A%252F%252Fmylearning.sumtotal.host%252Fcore%252FsearchRedirect%253FViewType%253DList%2526SearchText%253Dproblem%25252520handling%2526startRow%253D0%26SearchCallerID%3D2" xr:uid="{3F3444DB-7660-4A51-848B-83253AA886B2}"/>
-    <hyperlink ref="B3" r:id="rId4" display="https://mylearning.sumtotal.host/rcore/c/pillarRedirect?isDeepLink=1&amp;relyingParty=LM&amp;url=https%3A%2F%2Fmylearning.sumtotal.host%2Flearning%2Fcore%2Factivitydetails%2FViewActivityDetails%3FUserMode%3D0%26ActivityId%3D6635%26ClassUnderStruct%3DFalse%26CallerUrl%3D%2Flearning%2Flearner%2FHome%2FGoToPortal%3Fkey%3D0%26SearchCallerURL%3Dhttps%253A%252F%252Fmylearning.sumtotal.host%252Fcore%252FsearchRedirect%253FViewType%253DList%2526SearchText%253Dholiday%25252520inn%25252520express%25252520mission%25252520made%25252520easy%25252520brand%25252520orientation%2526startRow%253D0%26SearchCallerID%3D2" xr:uid="{2126190C-718B-438C-B0BE-FCD7F9179AB5}"/>
-    <hyperlink ref="B8" r:id="rId5" display="https://mylearning.sumtotal.host/rcore/c/pillarRedirect?isDeepLink=1&amp;relyingParty=LM&amp;url=https%3A%2F%2Fmylearning.sumtotal.host%2Flearning%2Fcore%2Factivitydetails%2FViewActivityDetails%3FUserMode%3D0%26ActivityId%3D564%26ClassUnderStruct%3DFalse%26CallerUrl%3D%2Flearning%2Flearner%2FHome%2FGoToPortal%3Fkey%3D0%26SearchCallerURL%3Dhttps%253A%252F%252Fmylearning.sumtotal.host%252Fcore%252FsearchRedirect%253FViewType%253DList%2526SearchText%253Dleading%25252520and%25252520sustaining%25252520your%25252520service%25252520culture%2526startRow%253D0%26SearchCallerID%3D2" xr:uid="{6DBDB61F-2E68-4EB9-B30F-00F29A7BF9F1}"/>
-    <hyperlink ref="B31" r:id="rId6" display="https://mylearning.sumtotal.host/rcore/c/pillarRedirect?isDeepLink=1&amp;relyingParty=LM&amp;url=https%3A%2F%2Fmylearning.sumtotal.host%2Flearning%2Fcore%2Factivitydetails%2FViewActivityDetails%3FUserMode%3D0%26ActivityId%3D5317%26ClassUnderStruct%3DFalse%26CallerUrl%3D%2Flearning%2Flearner%2FHome%2FGoToPortal%3Fkey%3D0%26SearchCallerURL%3Dhttps%253A%252F%252Fmylearning.sumtotal.host%252Fcore%252FsearchRedirect%253FViewType%253DList%2526SearchText%253Dway%25252520of%25252520sales%25252520solution%2526startRow%253D0%26SearchCallerID%3D2" xr:uid="{7A5E9469-F415-4D03-8F85-BDC532D61989}"/>
-    <hyperlink ref="B11" r:id="rId7" xr:uid="{98DDCFA9-C416-471C-9EDC-3027AC7F763F}"/>
-    <hyperlink ref="B13" r:id="rId8" xr:uid="{92F27482-CC2C-45C7-9D25-A770388E42D2}"/>
-    <hyperlink ref="B14" r:id="rId9" xr:uid="{5EB8CA66-65FA-402E-A4CF-3CB10B3A268F}"/>
-    <hyperlink ref="B15" r:id="rId10" xr:uid="{D2CD8E51-72AB-4BA6-9430-A01C8E8D8F23}"/>
-    <hyperlink ref="B16" r:id="rId11" xr:uid="{0AC8AC37-6EBD-4730-9B1F-ED466C1DBEA1}"/>
-    <hyperlink ref="B17" r:id="rId12" xr:uid="{0DB58F3E-37FC-4C0C-B7C2-37E4D91C1BB0}"/>
-    <hyperlink ref="B27" r:id="rId13" xr:uid="{B9137C61-945D-429A-ADE2-275E181D0582}"/>
-    <hyperlink ref="B26" r:id="rId14" xr:uid="{3CF3C093-BAD9-49AC-B05A-BC88BDEF5DCA}"/>
-    <hyperlink ref="B25" r:id="rId15" xr:uid="{EDBC6CFE-202B-4106-AF6E-8CE6F9904712}"/>
-    <hyperlink ref="B24" r:id="rId16" xr:uid="{F80219DB-4581-4297-B9B3-AE048131B026}"/>
-    <hyperlink ref="B23" r:id="rId17" xr:uid="{268940C4-B90A-4850-A710-95309CBD0E1C}"/>
-    <hyperlink ref="B22" r:id="rId18" xr:uid="{E404B77A-1778-4B43-858F-EBD27A5B81D5}"/>
-    <hyperlink ref="B21" r:id="rId19" xr:uid="{C926CCE4-2165-4E73-B551-725884C3172F}"/>
-    <hyperlink ref="B28" r:id="rId20" xr:uid="{1B92540F-FB4A-4483-A30D-C12B7A93F334}"/>
-    <hyperlink ref="B29" r:id="rId21" xr:uid="{ED60402C-18DD-4644-B01E-D0EA2DFD70C3}"/>
-    <hyperlink ref="B30" r:id="rId22" xr:uid="{8EB6F020-7B4B-4183-BEB9-A5230BF63EAC}"/>
-    <hyperlink ref="B32" r:id="rId23" xr:uid="{69852BC4-CA32-45E0-8396-4ADE53E9D611}"/>
-    <hyperlink ref="B33" r:id="rId24" xr:uid="{920E9061-78C7-45C6-8374-DD4880BF0EA6}"/>
-    <hyperlink ref="B19" r:id="rId25" xr:uid="{76059E5C-1D4C-44A6-BB1E-43F0EED855EA}"/>
-    <hyperlink ref="B20" r:id="rId26" xr:uid="{DE355AC0-1ADB-4BAE-B6BB-92E615D2DF06}"/>
-    <hyperlink ref="B5" r:id="rId27" xr:uid="{9B9521FF-AEE0-42BE-B7CE-8A9656BFE2EE}"/>
-    <hyperlink ref="B9" r:id="rId28" xr:uid="{8CEA093F-3038-46E9-A8E7-CDB3B8C5DBDD}"/>
-    <hyperlink ref="B12" r:id="rId29" xr:uid="{D1762190-A302-440C-9661-EAD2485056A6}"/>
-    <hyperlink ref="B38" r:id="rId30" xr:uid="{2CD8ABD7-011B-4DE4-8AA5-1F2EFD342B01}"/>
-    <hyperlink ref="B6" r:id="rId31" xr:uid="{B24AE84B-5ECA-49EE-AD12-EF798F34AC52}"/>
-    <hyperlink ref="B7" r:id="rId32" xr:uid="{D28EB901-777C-4D9C-8D17-22903421632A}"/>
-    <hyperlink ref="B34" r:id="rId33" xr:uid="{C0C1BBC3-2888-4A02-BE71-8FC941CF9088}"/>
-    <hyperlink ref="B35" r:id="rId34" xr:uid="{5FF31E64-A4F4-449D-9D61-CE67ED5300A0}"/>
-    <hyperlink ref="B36" r:id="rId35" xr:uid="{0990599C-42EA-4902-B929-A2BF7853DB55}"/>
-    <hyperlink ref="B4" r:id="rId36" xr:uid="{4A6DC263-9F86-43CD-800C-979CB229F1F5}"/>
-    <hyperlink ref="B41" r:id="rId37" xr:uid="{14FB1160-3545-4020-85D5-009A528BF6FD}"/>
+    <hyperlink ref="B17" r:id="rId2" xr:uid="{6307E43C-9BC0-489B-9BB5-E5C2004BE1F8}"/>
+    <hyperlink ref="B9" r:id="rId3" display="https://mylearning.sumtotal.host/rcore/c/pillarRedirect?isDeepLink=1&amp;relyingParty=LM&amp;url=https%3A%2F%2Fmylearning.sumtotal.host%2Flearning%2Fcore%2Factivitydetails%2FViewActivityDetails%3FUserMode%3D0%26ActivityId%3D21837%26ClassUnderStruct%3DFalse%26CallerUrl%3D%2Flearning%2Flearner%2FHome%2FGoToPortal%3Fkey%3D0%26SearchCallerURL%3Dhttps%253A%252F%252Fmylearning.sumtotal.host%252Fcore%252FsearchRedirect%253FViewType%253DList%2526SearchText%253Dproblem%25252520handling%2526startRow%253D0%26SearchCallerID%3D2" xr:uid="{3F3444DB-7660-4A51-848B-83253AA886B2}"/>
+    <hyperlink ref="B7" r:id="rId4" display="https://mylearning.sumtotal.host/rcore/c/pillarRedirect?isDeepLink=1&amp;relyingParty=LM&amp;url=https%3A%2F%2Fmylearning.sumtotal.host%2Flearning%2Fcore%2Factivitydetails%2FViewActivityDetails%3FUserMode%3D0%26ActivityId%3D564%26ClassUnderStruct%3DFalse%26CallerUrl%3D%2Flearning%2Flearner%2FHome%2FGoToPortal%3Fkey%3D0%26SearchCallerURL%3Dhttps%253A%252F%252Fmylearning.sumtotal.host%252Fcore%252FsearchRedirect%253FViewType%253DList%2526SearchText%253Dleading%25252520and%25252520sustaining%25252520your%25252520service%25252520culture%2526startRow%253D0%26SearchCallerID%3D2" xr:uid="{6DBDB61F-2E68-4EB9-B30F-00F29A7BF9F1}"/>
+    <hyperlink ref="B30" r:id="rId5" display="https://mylearning.sumtotal.host/rcore/c/pillarRedirect?isDeepLink=1&amp;relyingParty=LM&amp;url=https%3A%2F%2Fmylearning.sumtotal.host%2Flearning%2Fcore%2Factivitydetails%2FViewActivityDetails%3FUserMode%3D0%26ActivityId%3D5317%26ClassUnderStruct%3DFalse%26CallerUrl%3D%2Flearning%2Flearner%2FHome%2FGoToPortal%3Fkey%3D0%26SearchCallerURL%3Dhttps%253A%252F%252Fmylearning.sumtotal.host%252Fcore%252FsearchRedirect%253FViewType%253DList%2526SearchText%253Dway%25252520of%25252520sales%25252520solution%2526startRow%253D0%26SearchCallerID%3D2" xr:uid="{7A5E9469-F415-4D03-8F85-BDC532D61989}"/>
+    <hyperlink ref="B10" r:id="rId6" xr:uid="{98DDCFA9-C416-471C-9EDC-3027AC7F763F}"/>
+    <hyperlink ref="B12" r:id="rId7" xr:uid="{92F27482-CC2C-45C7-9D25-A770388E42D2}"/>
+    <hyperlink ref="B13" r:id="rId8" xr:uid="{5EB8CA66-65FA-402E-A4CF-3CB10B3A268F}"/>
+    <hyperlink ref="B14" r:id="rId9" xr:uid="{D2CD8E51-72AB-4BA6-9430-A01C8E8D8F23}"/>
+    <hyperlink ref="B15" r:id="rId10" xr:uid="{0AC8AC37-6EBD-4730-9B1F-ED466C1DBEA1}"/>
+    <hyperlink ref="B16" r:id="rId11" xr:uid="{0DB58F3E-37FC-4C0C-B7C2-37E4D91C1BB0}"/>
+    <hyperlink ref="B26" r:id="rId12" xr:uid="{B9137C61-945D-429A-ADE2-275E181D0582}"/>
+    <hyperlink ref="B25" r:id="rId13" xr:uid="{3CF3C093-BAD9-49AC-B05A-BC88BDEF5DCA}"/>
+    <hyperlink ref="B24" r:id="rId14" xr:uid="{EDBC6CFE-202B-4106-AF6E-8CE6F9904712}"/>
+    <hyperlink ref="B23" r:id="rId15" xr:uid="{F80219DB-4581-4297-B9B3-AE048131B026}"/>
+    <hyperlink ref="B22" r:id="rId16" xr:uid="{268940C4-B90A-4850-A710-95309CBD0E1C}"/>
+    <hyperlink ref="B21" r:id="rId17" xr:uid="{E404B77A-1778-4B43-858F-EBD27A5B81D5}"/>
+    <hyperlink ref="B20" r:id="rId18" xr:uid="{C926CCE4-2165-4E73-B551-725884C3172F}"/>
+    <hyperlink ref="B27" r:id="rId19" xr:uid="{1B92540F-FB4A-4483-A30D-C12B7A93F334}"/>
+    <hyperlink ref="B28" r:id="rId20" xr:uid="{ED60402C-18DD-4644-B01E-D0EA2DFD70C3}"/>
+    <hyperlink ref="B29" r:id="rId21" xr:uid="{8EB6F020-7B4B-4183-BEB9-A5230BF63EAC}"/>
+    <hyperlink ref="B31" r:id="rId22" xr:uid="{69852BC4-CA32-45E0-8396-4ADE53E9D611}"/>
+    <hyperlink ref="B32" r:id="rId23" xr:uid="{920E9061-78C7-45C6-8374-DD4880BF0EA6}"/>
+    <hyperlink ref="B18" r:id="rId24" xr:uid="{76059E5C-1D4C-44A6-BB1E-43F0EED855EA}"/>
+    <hyperlink ref="B19" r:id="rId25" xr:uid="{DE355AC0-1ADB-4BAE-B6BB-92E615D2DF06}"/>
+    <hyperlink ref="B4" r:id="rId26" xr:uid="{9B9521FF-AEE0-42BE-B7CE-8A9656BFE2EE}"/>
+    <hyperlink ref="B8" r:id="rId27" xr:uid="{8CEA093F-3038-46E9-A8E7-CDB3B8C5DBDD}"/>
+    <hyperlink ref="B11" r:id="rId28" xr:uid="{D1762190-A302-440C-9661-EAD2485056A6}"/>
+    <hyperlink ref="B37" r:id="rId29" xr:uid="{2CD8ABD7-011B-4DE4-8AA5-1F2EFD342B01}"/>
+    <hyperlink ref="B5" r:id="rId30" xr:uid="{B24AE84B-5ECA-49EE-AD12-EF798F34AC52}"/>
+    <hyperlink ref="B6" r:id="rId31" xr:uid="{D28EB901-777C-4D9C-8D17-22903421632A}"/>
+    <hyperlink ref="B33" r:id="rId32" xr:uid="{C0C1BBC3-2888-4A02-BE71-8FC941CF9088}"/>
+    <hyperlink ref="B34" r:id="rId33" xr:uid="{5FF31E64-A4F4-449D-9D61-CE67ED5300A0}"/>
+    <hyperlink ref="B35" r:id="rId34" xr:uid="{0990599C-42EA-4902-B929-A2BF7853DB55}"/>
+    <hyperlink ref="B3" r:id="rId35" xr:uid="{4A6DC263-9F86-43CD-800C-979CB229F1F5}"/>
+    <hyperlink ref="B40" r:id="rId36" xr:uid="{14FB1160-3545-4020-85D5-009A528BF6FD}"/>
+    <hyperlink ref="B36" r:id="rId37" xr:uid="{611DDFC6-6D15-45E4-BD46-FD513320F05C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6024,8 +5976,8 @@
   </sheetPr>
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8084,6 +8036,7 @@
     <hyperlink ref="B37" r:id="rId35" xr:uid="{6C4E488B-9E9C-47E5-8BCF-E365E757C2B8}"/>
     <hyperlink ref="B4" r:id="rId36" xr:uid="{145569E2-B0CA-41E0-A855-EB000EA14B8A}"/>
     <hyperlink ref="B5" r:id="rId37" xr:uid="{B39C3945-AA2A-4909-9DD5-750DB275A907}"/>
+    <hyperlink ref="B38" r:id="rId38" xr:uid="{BDB6DEFE-DBA9-4523-BF21-83EC574DF968}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8133,7 +8086,7 @@
   <dimension ref="A1:Q40"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10141,6 +10094,7 @@
     <hyperlink ref="B35" r:id="rId34" xr:uid="{78549E4E-D657-4D59-A26A-305DF0725EEE}"/>
     <hyperlink ref="B36" r:id="rId35" xr:uid="{881C5F22-1A0F-4980-B664-D43B656379DB}"/>
     <hyperlink ref="B4" r:id="rId36" xr:uid="{46907DBC-633E-43EF-B5E0-3FF6238C8871}"/>
+    <hyperlink ref="B37" r:id="rId37" xr:uid="{4391CB62-246A-4EB5-BA34-499C03AE9000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10155,7 +10109,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12273,6 +12227,7 @@
     <hyperlink ref="B35" r:id="rId35" xr:uid="{C137CC9E-9E6A-4BE9-A6A7-8D461B774052}"/>
     <hyperlink ref="B36" r:id="rId36" xr:uid="{930AE9EE-C36D-4BF2-A28A-69DFA5F4D518}"/>
     <hyperlink ref="B37" r:id="rId37" xr:uid="{7DA7EB5D-163B-469E-B5E1-BA228BB5FD50}"/>
+    <hyperlink ref="B38" r:id="rId38" xr:uid="{1318B36D-A1A2-4B6E-B818-6997DD25D96C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12285,8 +12240,8 @@
   </sheetPr>
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14293,6 +14248,7 @@
     <hyperlink ref="B35" r:id="rId34" xr:uid="{35F8F9BD-A805-4896-9894-333D645E037D}"/>
     <hyperlink ref="B36" r:id="rId35" xr:uid="{B8EEEC4E-0421-4D4E-B078-E1086193B719}"/>
     <hyperlink ref="B4" r:id="rId36" xr:uid="{BB0F75FC-BF8B-4E19-93F8-948064D07D38}"/>
+    <hyperlink ref="B37" r:id="rId37" xr:uid="{4C219508-B9EE-4C50-887E-C0F36FB31AD7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14305,8 +14261,8 @@
   </sheetPr>
   <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -16366,23 +16322,23 @@
       <c r="Q43" s="91"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" s="108"/>
-      <c r="B44" s="108"/>
-      <c r="C44" s="108"/>
-      <c r="D44" s="108"/>
-      <c r="E44" s="108"/>
-      <c r="F44" s="108"/>
-      <c r="G44" s="108"/>
-      <c r="H44" s="108"/>
-      <c r="I44" s="108"/>
-      <c r="J44" s="108"/>
-      <c r="K44" s="108"/>
-      <c r="L44" s="108"/>
-      <c r="M44" s="108"/>
-      <c r="N44" s="108"/>
-      <c r="O44" s="108"/>
-      <c r="P44" s="108"/>
-      <c r="Q44" s="108"/>
+      <c r="A44" s="109"/>
+      <c r="B44" s="109"/>
+      <c r="C44" s="109"/>
+      <c r="D44" s="109"/>
+      <c r="E44" s="109"/>
+      <c r="F44" s="109"/>
+      <c r="G44" s="109"/>
+      <c r="H44" s="109"/>
+      <c r="I44" s="109"/>
+      <c r="J44" s="109"/>
+      <c r="K44" s="109"/>
+      <c r="L44" s="109"/>
+      <c r="M44" s="109"/>
+      <c r="N44" s="109"/>
+      <c r="O44" s="109"/>
+      <c r="P44" s="109"/>
+      <c r="Q44" s="109"/>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="86"/>
@@ -16464,6 +16420,7 @@
     <hyperlink ref="B37" r:id="rId35" xr:uid="{C588DE9B-15F9-4160-BEC9-DEAF369DDBF9}"/>
     <hyperlink ref="B4" r:id="rId36" display="https://mylearning.sumtotal.host/rcore/c/pillarRedirect?isDeepLink=1&amp;relyingParty=LM&amp;url=https%3A%2F%2Fmylearning.sumtotal.host%2Flearning%2Fcore%2Factivitydetails%2FViewActivityDetails%3FUserMode%3D0%26ActivityId%3D10778%26ClassUnderStruct%3DFalse%26CallerUrl%3D%2Flearning%2Flearner%2FHome%2FGoToPortal%3Fkey%3D0%26SearchCallerURL%3Dhttps%253A%252F%252Fmylearning.sumtotal.host%252Fcore%252FsearchRedirect%253FViewType%253DList%2526SearchText%253Dbrand%25252520orientation%2526startRow%253D0%26SearchCallerID%3D2" xr:uid="{5C80622A-0320-4322-A207-415378A8E922}"/>
     <hyperlink ref="B5" r:id="rId37" display="https://mylearning.sumtotal.host/rcore/c/pillarRedirect?isDeepLink=1&amp;relyingParty=LM&amp;url=https%3A%2F%2Fmylearning.sumtotal.host%2Flearning%2Fcore%2Factivitydetails%2FViewActivityDetails%3FUserMode%3D0%26ActivityId%3D10779%26ClassUnderStruct%3DFalse%26CallerUrl%3D%2Flearning%2Flearner%2FHome%2FGoToPortal%3Fkey%3D0%26SearchCallerURL%3Dhttps%253A%252F%252Fmylearning.sumtotal.host%252Fcore%252FsearchRedirect%253FViewType%253DList%2526SearchText%253Dbrand%25252520experience%2526startRow%253D0%26SearchCallerID%3D2" xr:uid="{F95AD6C1-C976-46D3-B90C-59C3FFE68FF5}"/>
+    <hyperlink ref="B38" r:id="rId38" xr:uid="{8F100AB9-DBBE-4491-804C-83964F68C323}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16476,8 +16433,8 @@
   </sheetPr>
   <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -18306,7 +18263,7 @@
       <c r="A38" s="101" t="s">
         <v>137</v>
       </c>
-      <c r="B38" s="102" t="s">
+      <c r="B38" s="108" t="s">
         <v>138</v>
       </c>
       <c r="C38" s="102"/>
@@ -18653,6 +18610,7 @@
     <hyperlink ref="B43" r:id="rId39" xr:uid="{A34C86DB-8DE0-4C7C-84ED-737E2DE1B7AF}"/>
     <hyperlink ref="B44" r:id="rId40" xr:uid="{E93D3E41-FAA8-40CB-8C93-7EFCE0039966}"/>
     <hyperlink ref="B45" r:id="rId41" xr:uid="{5867F5DD-3A7D-410E-A420-A78570FD590C}"/>
+    <hyperlink ref="B38" r:id="rId42" xr:uid="{C564AAF7-5F80-4F9D-86A7-919FD74720E1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18665,8 +18623,8 @@
   </sheetPr>
   <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -20978,6 +20936,7 @@
     <hyperlink ref="B44" r:id="rId40" xr:uid="{922EC4E3-1526-45E6-B6AB-FD0220848034}"/>
     <hyperlink ref="B45" r:id="rId41" xr:uid="{3B3EF3A5-FC18-4D4E-AAC2-4497E23849D9}"/>
     <hyperlink ref="B46" r:id="rId42" xr:uid="{E70F4F0B-2825-47C7-A9BA-0ACD52E504F1}"/>
+    <hyperlink ref="B39" r:id="rId43" xr:uid="{FDFED488-AD79-4FFA-890F-F552C5AFED9A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20990,8 +20949,8 @@
   </sheetPr>
   <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23169,9 +23128,10 @@
     <hyperlink ref="B43" r:id="rId39" xr:uid="{2FBFD48A-0D2A-4122-BF3E-DF4525F9CFA9}"/>
     <hyperlink ref="B44" r:id="rId40" xr:uid="{A41C8ED4-3FE2-4746-AD94-10AB3A672865}"/>
     <hyperlink ref="B45" r:id="rId41" xr:uid="{B1031242-5C3A-4514-9450-6DF91C09016B}"/>
+    <hyperlink ref="B38" r:id="rId42" xr:uid="{C2DFCA5D-2652-4468-A819-E2CC21A5F40A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="17" orientation="portrait" r:id="rId42"/>
+  <pageSetup paperSize="17" orientation="portrait" r:id="rId43"/>
 </worksheet>
 </file>
 
@@ -23182,8 +23142,8 @@
   </sheetPr>
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25238,6 +25198,7 @@
     <hyperlink ref="B35" r:id="rId34" xr:uid="{95FAB6D9-1AE8-458B-A8E1-8AEC8392BEAE}"/>
     <hyperlink ref="B36" r:id="rId35" xr:uid="{BFA7015C-0094-43E2-9B37-42B997706AEB}"/>
     <hyperlink ref="B4" r:id="rId36" xr:uid="{24BEFA0D-8CAB-4A22-B4C4-2EFBC2AA53B3}"/>
+    <hyperlink ref="B37" r:id="rId37" xr:uid="{AA61CD7D-E757-466B-B069-71D25EE00C5F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -25250,8 +25211,8 @@
   </sheetPr>
   <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView topLeftCell="C34" workbookViewId="0">
-      <selection activeCell="Q46" sqref="Q46"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27412,6 +27373,7 @@
     <hyperlink ref="B4" r:id="rId36" xr:uid="{5AB798A6-C74D-4C72-8014-564314A5B07B}"/>
     <hyperlink ref="B5" r:id="rId37" xr:uid="{9946A213-D932-4C76-926B-730D4C0D543A}"/>
     <hyperlink ref="B42" r:id="rId38" xr:uid="{8736C589-6FF2-4688-948F-65AB3A8CEA66}"/>
+    <hyperlink ref="B38" r:id="rId39" xr:uid="{A609D14D-E356-43FA-9FA3-7263F303BE43}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>